<commit_message>
now it work as long as excel file (data.xlsx) in the same folder
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -505,7 +505,7 @@
       <selection activeCell="B201" sqref="B201"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
     <col width="83.109375" customWidth="1" min="2" max="2"/>
     <col width="14.109375" customWidth="1" min="3" max="3"/>
@@ -3712,7 +3712,7 @@
         </is>
       </c>
       <c r="C200" s="8" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D200" s="8" t="n">
         <v>2</v>

</xml_diff>

<commit_message>
Now it can Change name, create new ID if not found along with Guests Count, Sum USD, Sum Riel
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -103,7 +103,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -121,6 +121,10 @@
     <xf numFmtId="165" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -499,21 +503,22 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D385"/>
+  <dimension ref="A1:D272"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B201" sqref="B201"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="B69" sqref="B69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col width="83.109375" customWidth="1" min="2" max="2"/>
-    <col width="14.109375" customWidth="1" min="3" max="3"/>
-    <col width="15" customWidth="1" min="4" max="4"/>
+    <col width="9.140625" customWidth="1" style="12" min="1" max="1"/>
+    <col width="83.140625" customWidth="1" min="2" max="2"/>
+    <col width="14.140625" customWidth="1" style="10" min="3" max="3"/>
+    <col width="15" customWidth="1" style="10" min="4" max="4"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="4" t="inlineStr">
+      <c r="A1" s="11" t="inlineStr">
         <is>
           <t>ID</t>
         </is>
@@ -523,12 +528,12 @@
           <t>Name</t>
         </is>
       </c>
-      <c r="C1" s="4" t="inlineStr">
+      <c r="C1" s="9" t="inlineStr">
         <is>
           <t>USD</t>
         </is>
       </c>
-      <c r="D1" s="4" t="inlineStr">
+      <c r="D1" s="9" t="inlineStr">
         <is>
           <t>Riel</t>
         </is>
@@ -544,7 +549,7 @@
         </is>
       </c>
       <c r="C2" s="8" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D2" s="8" t="n">
         <v>0</v>
@@ -563,7 +568,7 @@
         <v>0</v>
       </c>
       <c r="D3" s="8" t="n">
-        <v>0</v>
+        <v>3454</v>
       </c>
     </row>
     <row r="4" ht="18.75" customHeight="1">
@@ -579,7 +584,7 @@
         <v>0</v>
       </c>
       <c r="D4" s="8" t="n">
-        <v>0</v>
+        <v>345</v>
       </c>
     </row>
     <row r="5" ht="18.75" customHeight="1">
@@ -592,7 +597,7 @@
         </is>
       </c>
       <c r="C5" s="8" t="n">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="D5" s="8" t="n">
         <v>0</v>
@@ -4855,918 +4860,134 @@
       </c>
     </row>
     <row r="272" ht="18" customHeight="1">
-      <c r="C272" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D272" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="273" ht="18" customHeight="1">
-      <c r="C273" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D273" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="274" ht="18" customHeight="1">
-      <c r="C274" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D274" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="275" ht="18" customHeight="1">
-      <c r="C275" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D275" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="276" ht="18" customHeight="1">
-      <c r="C276" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D276" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="277" ht="18" customHeight="1">
-      <c r="C277" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D277" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="278" ht="18" customHeight="1">
-      <c r="C278" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D278" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="279" ht="18" customHeight="1">
-      <c r="C279" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D279" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="280" ht="18" customHeight="1">
-      <c r="C280" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D280" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="281" ht="18" customHeight="1">
-      <c r="C281" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D281" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="282" ht="18" customHeight="1">
-      <c r="C282" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D282" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="283" ht="18" customHeight="1">
-      <c r="C283" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D283" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="284" ht="18" customHeight="1">
-      <c r="C284" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D284" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="285" ht="18" customHeight="1">
-      <c r="C285" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D285" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="286" ht="18" customHeight="1">
-      <c r="C286" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D286" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="287" ht="18" customHeight="1">
-      <c r="C287" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D287" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="288" ht="18" customHeight="1">
-      <c r="C288" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D288" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="289" ht="18" customHeight="1">
-      <c r="C289" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D289" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="290" ht="18" customHeight="1">
-      <c r="C290" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D290" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="291" ht="18" customHeight="1">
-      <c r="C291" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D291" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="292" ht="18" customHeight="1">
-      <c r="C292" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D292" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="293" ht="18" customHeight="1">
-      <c r="C293" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D293" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="294" ht="18" customHeight="1">
-      <c r="C294" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D294" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="295" ht="18" customHeight="1">
-      <c r="C295" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D295" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="296" ht="18" customHeight="1">
-      <c r="C296" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D296" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="297" ht="18" customHeight="1">
-      <c r="C297" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D297" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="298" ht="18" customHeight="1">
-      <c r="C298" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D298" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="299" ht="18" customHeight="1">
-      <c r="C299" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D299" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="300" ht="18" customHeight="1">
-      <c r="C300" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D300" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="301" ht="18" customHeight="1">
-      <c r="C301" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D301" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="302" ht="18" customHeight="1">
-      <c r="C302" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D302" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="303" ht="18" customHeight="1">
-      <c r="C303" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D303" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="304" ht="18" customHeight="1">
-      <c r="C304" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D304" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="305" ht="18" customHeight="1">
-      <c r="C305" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D305" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="306" ht="18" customHeight="1">
-      <c r="C306" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D306" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="307" ht="18" customHeight="1">
-      <c r="C307" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D307" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="308" ht="18" customHeight="1">
-      <c r="C308" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D308" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="309" ht="18" customHeight="1">
-      <c r="C309" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D309" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="310" ht="18" customHeight="1">
-      <c r="C310" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D310" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="311" ht="18" customHeight="1">
-      <c r="C311" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D311" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="312" ht="18" customHeight="1">
-      <c r="C312" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D312" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="313" ht="18" customHeight="1">
-      <c r="C313" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D313" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="314" ht="18" customHeight="1">
-      <c r="C314" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D314" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="315" ht="18" customHeight="1">
-      <c r="C315" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D315" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="316" ht="18" customHeight="1">
-      <c r="C316" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D316" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="317" ht="18" customHeight="1">
-      <c r="C317" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D317" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="318" ht="18" customHeight="1">
-      <c r="C318" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D318" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="319" ht="18" customHeight="1">
-      <c r="C319" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D319" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="320" ht="18" customHeight="1">
-      <c r="C320" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D320" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="321" ht="18" customHeight="1">
-      <c r="C321" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D321" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="322" ht="18" customHeight="1">
-      <c r="C322" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D322" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="323" ht="18" customHeight="1">
-      <c r="C323" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D323" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="324" ht="18" customHeight="1">
-      <c r="C324" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D324" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="325" ht="18" customHeight="1">
-      <c r="C325" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D325" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="326" ht="18" customHeight="1">
-      <c r="C326" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D326" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="327" ht="18" customHeight="1">
-      <c r="C327" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D327" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="328" ht="18" customHeight="1">
-      <c r="C328" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D328" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="329" ht="18" customHeight="1">
-      <c r="C329" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D329" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="330" ht="18" customHeight="1">
-      <c r="C330" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D330" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="331" ht="18" customHeight="1">
-      <c r="C331" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D331" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="332" ht="18" customHeight="1">
-      <c r="C332" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D332" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="333" ht="18" customHeight="1">
-      <c r="C333" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D333" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="334" ht="18" customHeight="1">
-      <c r="C334" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D334" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="335" ht="18" customHeight="1">
-      <c r="C335" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D335" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="336" ht="18" customHeight="1">
-      <c r="C336" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D336" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="337" ht="18" customHeight="1">
-      <c r="C337" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D337" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="338" ht="18" customHeight="1">
-      <c r="C338" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D338" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="339" ht="18" customHeight="1">
-      <c r="C339" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D339" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="340" ht="18" customHeight="1">
-      <c r="C340" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D340" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="341" ht="18" customHeight="1">
-      <c r="C341" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D341" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="342" ht="18" customHeight="1">
-      <c r="C342" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D342" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="343" ht="18" customHeight="1">
-      <c r="C343" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D343" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="344" ht="18" customHeight="1">
-      <c r="C344" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D344" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="345" ht="18" customHeight="1">
-      <c r="C345" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D345" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="346" ht="18" customHeight="1">
-      <c r="C346" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D346" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="347" ht="18" customHeight="1">
-      <c r="C347" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D347" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="348" ht="18" customHeight="1">
-      <c r="C348" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D348" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="349" ht="18" customHeight="1">
-      <c r="C349" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D349" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="350" ht="18" customHeight="1">
-      <c r="C350" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D350" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="351" ht="18" customHeight="1">
-      <c r="C351" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D351" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="352" ht="18" customHeight="1">
-      <c r="C352" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D352" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="353" ht="18" customHeight="1">
-      <c r="C353" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D353" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="354" ht="18" customHeight="1">
-      <c r="C354" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D354" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="355" ht="18" customHeight="1">
-      <c r="C355" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D355" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="356" ht="18" customHeight="1">
-      <c r="C356" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D356" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="357" ht="18" customHeight="1">
-      <c r="C357" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D357" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="358" ht="18" customHeight="1">
-      <c r="C358" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D358" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="359" ht="18" customHeight="1">
-      <c r="C359" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D359" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="360" ht="18" customHeight="1">
-      <c r="C360" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D360" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="361" ht="18" customHeight="1">
-      <c r="C361" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D361" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="362" ht="18" customHeight="1">
-      <c r="C362" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D362" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="363" ht="18" customHeight="1">
-      <c r="C363" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D363" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="364" ht="18" customHeight="1">
-      <c r="C364" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D364" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="365" ht="18" customHeight="1">
-      <c r="C365" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D365" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="366" ht="18" customHeight="1">
-      <c r="C366" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D366" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="367" ht="18" customHeight="1">
-      <c r="C367" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D367" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="368" ht="18" customHeight="1">
-      <c r="C368" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D368" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="369" ht="18" customHeight="1">
-      <c r="C369" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D369" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="370" ht="18" customHeight="1">
-      <c r="C370" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D370" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="371" ht="18" customHeight="1">
-      <c r="C371" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D371" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="372" ht="18" customHeight="1">
-      <c r="C372" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D372" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="373" ht="18" customHeight="1">
-      <c r="C373" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D373" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="374" ht="18" customHeight="1">
-      <c r="C374" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D374" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="375" ht="18" customHeight="1">
-      <c r="C375" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D375" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="376" ht="18" customHeight="1">
-      <c r="C376" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D376" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="377" ht="18" customHeight="1">
-      <c r="C377" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D377" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="378" ht="18" customHeight="1">
-      <c r="C378" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D378" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="379" ht="18" customHeight="1">
-      <c r="C379" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D379" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="380" ht="18" customHeight="1">
-      <c r="C380" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D380" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="381" ht="18" customHeight="1">
-      <c r="C381" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D381" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="382" ht="18" customHeight="1">
-      <c r="C382" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D382" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="383" ht="18" customHeight="1">
-      <c r="C383" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D383" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="384" ht="18" customHeight="1">
-      <c r="C384" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D384" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="385" ht="18" customHeight="1">
-      <c r="C385" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D385" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
+      <c r="A272" t="inlineStr">
+        <is>
+          <t>000</t>
+        </is>
+      </c>
+      <c r="B272" t="inlineStr"/>
+      <c r="C272" t="n">
+        <v>0</v>
+      </c>
+      <c r="D272" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="273" ht="18" customHeight="1"/>
+    <row r="274" ht="18" customHeight="1"/>
+    <row r="275" ht="18" customHeight="1"/>
+    <row r="276" ht="18" customHeight="1"/>
+    <row r="277" ht="18" customHeight="1"/>
+    <row r="278" ht="18" customHeight="1"/>
+    <row r="279" ht="18" customHeight="1"/>
+    <row r="280" ht="18" customHeight="1"/>
+    <row r="281" ht="18" customHeight="1"/>
+    <row r="282" ht="18" customHeight="1"/>
+    <row r="283" ht="18" customHeight="1"/>
+    <row r="284" ht="18" customHeight="1"/>
+    <row r="285" ht="18" customHeight="1"/>
+    <row r="286" ht="18" customHeight="1"/>
+    <row r="287" ht="18" customHeight="1"/>
+    <row r="288" ht="18" customHeight="1"/>
+    <row r="289" ht="18" customHeight="1"/>
+    <row r="290" ht="18" customHeight="1"/>
+    <row r="291" ht="18" customHeight="1"/>
+    <row r="292" ht="18" customHeight="1"/>
+    <row r="293" ht="18" customHeight="1"/>
+    <row r="294" ht="18" customHeight="1"/>
+    <row r="295" ht="18" customHeight="1"/>
+    <row r="296" ht="18" customHeight="1"/>
+    <row r="297" ht="18" customHeight="1"/>
+    <row r="298" ht="18" customHeight="1"/>
+    <row r="299" ht="18" customHeight="1"/>
+    <row r="300" ht="18" customHeight="1"/>
+    <row r="301" ht="18" customHeight="1"/>
+    <row r="302" ht="18" customHeight="1"/>
+    <row r="303" ht="18" customHeight="1"/>
+    <row r="304" ht="18" customHeight="1"/>
+    <row r="305" ht="18" customHeight="1"/>
+    <row r="306" ht="18" customHeight="1"/>
+    <row r="307" ht="18" customHeight="1"/>
+    <row r="308" ht="18" customHeight="1"/>
+    <row r="309" ht="18" customHeight="1"/>
+    <row r="310" ht="18" customHeight="1"/>
+    <row r="311" ht="18" customHeight="1"/>
+    <row r="312" ht="18" customHeight="1"/>
+    <row r="313" ht="18" customHeight="1"/>
+    <row r="314" ht="18" customHeight="1"/>
+    <row r="315" ht="18" customHeight="1"/>
+    <row r="316" ht="18" customHeight="1"/>
+    <row r="317" ht="18" customHeight="1"/>
+    <row r="318" ht="18" customHeight="1"/>
+    <row r="319" ht="18" customHeight="1"/>
+    <row r="320" ht="18" customHeight="1"/>
+    <row r="321" ht="18" customHeight="1"/>
+    <row r="322" ht="18" customHeight="1"/>
+    <row r="323" ht="18" customHeight="1"/>
+    <row r="324" ht="18" customHeight="1"/>
+    <row r="325" ht="18" customHeight="1"/>
+    <row r="326" ht="18" customHeight="1"/>
+    <row r="327" ht="18" customHeight="1"/>
+    <row r="328" ht="18" customHeight="1"/>
+    <row r="329" ht="18" customHeight="1"/>
+    <row r="330" ht="18" customHeight="1"/>
+    <row r="331" ht="18" customHeight="1"/>
+    <row r="332" ht="18" customHeight="1"/>
+    <row r="333" ht="18" customHeight="1"/>
+    <row r="334" ht="18" customHeight="1"/>
+    <row r="335" ht="18" customHeight="1"/>
+    <row r="336" ht="18" customHeight="1"/>
+    <row r="337" ht="18" customHeight="1"/>
+    <row r="338" ht="18" customHeight="1"/>
+    <row r="339" ht="18" customHeight="1"/>
+    <row r="340" ht="18" customHeight="1"/>
+    <row r="341" ht="18" customHeight="1"/>
+    <row r="342" ht="18" customHeight="1"/>
+    <row r="343" ht="18" customHeight="1"/>
+    <row r="344" ht="18" customHeight="1"/>
+    <row r="345" ht="18" customHeight="1"/>
+    <row r="346" ht="18" customHeight="1"/>
+    <row r="347" ht="18" customHeight="1"/>
+    <row r="348" ht="18" customHeight="1"/>
+    <row r="349" ht="18" customHeight="1"/>
+    <row r="350" ht="18" customHeight="1"/>
+    <row r="351" ht="18" customHeight="1"/>
+    <row r="352" ht="18" customHeight="1"/>
+    <row r="353" ht="18" customHeight="1"/>
+    <row r="354" ht="18" customHeight="1"/>
+    <row r="355" ht="18" customHeight="1"/>
+    <row r="356" ht="18" customHeight="1"/>
+    <row r="357" ht="18" customHeight="1"/>
+    <row r="358" ht="18" customHeight="1"/>
+    <row r="359" ht="18" customHeight="1"/>
+    <row r="360" ht="18" customHeight="1"/>
+    <row r="361" ht="18" customHeight="1"/>
+    <row r="362" ht="18" customHeight="1"/>
+    <row r="363" ht="18" customHeight="1"/>
+    <row r="364" ht="18" customHeight="1"/>
+    <row r="365" ht="18" customHeight="1"/>
+    <row r="366" ht="18" customHeight="1"/>
+    <row r="367" ht="18" customHeight="1"/>
+    <row r="368" ht="18" customHeight="1"/>
+    <row r="369" ht="18" customHeight="1"/>
+    <row r="370" ht="18" customHeight="1"/>
+    <row r="371" ht="18" customHeight="1"/>
+    <row r="372" ht="18" customHeight="1"/>
+    <row r="373" ht="18" customHeight="1"/>
+    <row r="374" ht="18" customHeight="1"/>
+    <row r="375" ht="18" customHeight="1"/>
+    <row r="376" ht="18" customHeight="1"/>
+    <row r="377" ht="18" customHeight="1"/>
+    <row r="378" ht="18" customHeight="1"/>
+    <row r="379" ht="18" customHeight="1"/>
+    <row r="380" ht="18" customHeight="1"/>
+    <row r="381" ht="18" customHeight="1"/>
+    <row r="382" ht="18" customHeight="1"/>
+    <row r="383" ht="18" customHeight="1"/>
+    <row r="384" ht="18" customHeight="1"/>
+    <row r="385" ht="18" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>